<commit_message>
refactor of VfM analysis. Workin. Ready for initial user testing
</commit_message>
<xml_diff>
--- a/tests/resources/vfm.xlsx
+++ b/tests/resources/vfm.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Q1_20_21" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Q4_19_20" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Count" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -355,6 +356,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Project/Programme</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>NPV for all projects and NPV for programmes if available</t>
@@ -538,6 +544,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Project/Programme</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>NPV for all projects and NPV for programmes if available</t>
@@ -706,6 +717,281 @@
       </c>
       <c r="H8" t="n">
         <v>738.36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B2:D23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>PVC total per category</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Q1 20/21</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Q4 19/20</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Poor</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>1172</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>2956</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2831</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>1761</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Very High</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>2089</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1481.6</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Very High and Financially Positive</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Economically Positive</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>7978</v>
+      </c>
+      <c r="D11" t="n">
+        <v>7245.6</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Category count</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Q1 20/21</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Q4 19/20</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Poor</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>2</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Very High</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Very High and Financially Positive</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Economically Positive</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>5</v>
+      </c>
+      <c r="D23" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
further optionality for vfm. Master update to use project abbreviations earlier
</commit_message>
<xml_diff>
--- a/tests/resources/vfm.xlsx
+++ b/tests/resources/vfm.xlsx
@@ -347,7 +347,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:K7"/>
+  <dimension ref="B2:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -410,168 +410,75 @@
     <row r="3">
       <c r="B3" t="inlineStr">
         <is>
-          <t>Mars</t>
+          <t>SoT</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>28369</v>
+        <v>1469.2</v>
       </c>
       <c r="D3" t="n">
-        <v>14.58</v>
+        <v>2.58</v>
       </c>
       <c r="E3" t="n">
-        <v>12.98</v>
+        <v>1.36</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Very High</t>
+          <t>High</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Very High</t>
+          <t>High</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Very High</t>
+          <t>High</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>2089</v>
+        <v>928</v>
       </c>
       <c r="J3" t="n">
-        <v>30458</v>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">All you need is love, love is all you need </t>
-        </is>
+        <v>2398</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>SoT</t>
+          <t>F9</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1469.2</v>
+        <v>1356</v>
       </c>
       <c r="D4" t="n">
-        <v>2.58</v>
+        <v>1.46</v>
       </c>
       <c r="E4" t="n">
-        <v>1.36</v>
+        <v>0.74</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>928</v>
+        <v>2956</v>
       </c>
       <c r="J4" t="n">
-        <v>2398</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>A13</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>1985</v>
-      </c>
-      <c r="D5" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="E5" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>833</v>
-      </c>
-      <c r="J5" t="n">
-        <v>3494</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>F9</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>1356</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1.46</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.74</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>2956</v>
-      </c>
-      <c r="J6" t="n">
         <v>4312</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Columbia</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>0.38</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.63</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Poor</t>
-        </is>
-      </c>
-      <c r="I7" t="n">
-        <v>1172</v>
-      </c>
-      <c r="J7" t="n">
-        <v>738.36</v>
       </c>
     </row>
   </sheetData>
@@ -585,7 +492,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:K8"/>
+  <dimension ref="B2:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -648,49 +555,49 @@
     <row r="3">
       <c r="B3" t="inlineStr">
         <is>
-          <t>Mars</t>
+          <t>SoT</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>30292.2</v>
+        <v>1469.2</v>
       </c>
       <c r="D3" t="n">
-        <v>21.45</v>
+        <v>2.58</v>
       </c>
       <c r="E3" t="n">
-        <v>19.72</v>
+        <v>1.36</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Very High</t>
+          <t>High</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>1481.6</v>
+        <v>928</v>
       </c>
       <c r="J3" t="n">
-        <v>31773.8</v>
+        <v>2398</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Hello is it me you’re looking for</t>
+          <t>Please allow me to introduce myself I’m a man of wealth and taste.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>SoT</t>
+          <t>A13</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1469.2</v>
+        <v>1985</v>
       </c>
       <c r="D4" t="n">
-        <v>2.58</v>
+        <v>2.3</v>
       </c>
       <c r="E4" t="n">
-        <v>1.36</v>
+        <v>2.3</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -698,99 +605,33 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>928</v>
+        <v>833</v>
       </c>
       <c r="J4" t="n">
-        <v>2398</v>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Please allow me to introduce myself I’m a man of wealth and taste.</t>
-        </is>
+        <v>3494</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="inlineStr">
         <is>
-          <t>A11</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>A13</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>1985</v>
-      </c>
-      <c r="D6" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="E6" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>833</v>
-      </c>
-      <c r="J6" t="n">
-        <v>3494</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>F9</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>2952</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1.54</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="I7" t="n">
-        <v>2831</v>
-      </c>
-      <c r="J7" t="n">
-        <v>4364</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" t="inlineStr">
-        <is>
           <t>Columbia</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="D5" t="n">
         <v>0.38</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E5" t="n">
         <v>0.63</v>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>Poor</t>
         </is>
       </c>
-      <c r="I8" t="n">
+      <c r="I5" t="n">
         <v>1172</v>
       </c>
-      <c r="J8" t="n">
+      <c r="J5" t="n">
         <v>738.36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
optionality/kwargs for vfm moved into VfMData class. vfm tests passing
</commit_message>
<xml_diff>
--- a/tests/resources/vfm.xlsx
+++ b/tests/resources/vfm.xlsx
@@ -347,7 +347,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:K4"/>
+  <dimension ref="B2:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -410,75 +410,168 @@
     <row r="3">
       <c r="B3" t="inlineStr">
         <is>
-          <t>SoT</t>
+          <t>Mars</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1469.2</v>
+        <v>28369</v>
       </c>
       <c r="D3" t="n">
-        <v>2.58</v>
+        <v>14.58</v>
       </c>
       <c r="E3" t="n">
-        <v>1.36</v>
+        <v>12.98</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Very High</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Very High</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Very High</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>928</v>
+        <v>2089</v>
       </c>
       <c r="J3" t="n">
-        <v>2398</v>
+        <v>30458</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">All you need is love, love is all you need </t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>F9</t>
+          <t>Sea of Tranquility</t>
         </is>
       </c>
       <c r="C4" t="n">
+        <v>1469.2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2.58</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>928</v>
+      </c>
+      <c r="J4" t="n">
+        <v>2398</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Apollo 13</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1985</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>833</v>
+      </c>
+      <c r="J5" t="n">
+        <v>3494</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Falcon 9</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
         <v>1356</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D6" t="n">
         <v>1.46</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E6" t="n">
         <v>0.74</v>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>N/A</t>
         </is>
       </c>
-      <c r="I4" t="n">
+      <c r="I6" t="n">
         <v>2956</v>
       </c>
-      <c r="J4" t="n">
+      <c r="J6" t="n">
         <v>4312</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Columbia</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Poor</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>1172</v>
+      </c>
+      <c r="J7" t="n">
+        <v>738.36</v>
       </c>
     </row>
   </sheetData>
@@ -492,7 +585,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:K5"/>
+  <dimension ref="B2:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -555,49 +648,49 @@
     <row r="3">
       <c r="B3" t="inlineStr">
         <is>
-          <t>SoT</t>
+          <t>Mars</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1469.2</v>
+        <v>30292.2</v>
       </c>
       <c r="D3" t="n">
-        <v>2.58</v>
+        <v>21.45</v>
       </c>
       <c r="E3" t="n">
-        <v>1.36</v>
+        <v>19.72</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Very High</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>928</v>
+        <v>1481.6</v>
       </c>
       <c r="J3" t="n">
-        <v>2398</v>
+        <v>31773.8</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Please allow me to introduce myself I’m a man of wealth and taste.</t>
+          <t>Hello is it me you’re looking for</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>A13</t>
+          <t>Sea of Tranquility</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1985</v>
+        <v>1469.2</v>
       </c>
       <c r="D4" t="n">
-        <v>2.3</v>
+        <v>2.58</v>
       </c>
       <c r="E4" t="n">
-        <v>2.3</v>
+        <v>1.36</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -605,33 +698,99 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>833</v>
+        <v>928</v>
       </c>
       <c r="J4" t="n">
-        <v>3494</v>
+        <v>2398</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Please allow me to introduce myself I’m a man of wealth and taste.</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="inlineStr">
         <is>
+          <t>Apollo 11</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Apollo 13</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1985</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>833</v>
+      </c>
+      <c r="J6" t="n">
+        <v>3494</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Falcon 9</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>2952</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="I7" t="n">
+        <v>2831</v>
+      </c>
+      <c r="J7" t="n">
+        <v>4364</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="inlineStr">
+        <is>
           <t>Columbia</t>
         </is>
       </c>
-      <c r="D5" t="n">
+      <c r="D8" t="n">
         <v>0.38</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E8" t="n">
         <v>0.63</v>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>Poor</t>
         </is>
       </c>
-      <c r="I5" t="n">
+      <c r="I8" t="n">
         <v>1172</v>
       </c>
-      <c r="J5" t="n">
+      <c r="J8" t="n">
         <v>738.36</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cost analysis in cli first commit. start of group/quarter structure to CostData class. change dft group rdm to rpe
</commit_message>
<xml_diff>
--- a/tests/resources/vfm.xlsx
+++ b/tests/resources/vfm.xlsx
@@ -347,7 +347,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:K5"/>
+  <dimension ref="B2:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,61 +449,24 @@
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>F9</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1356</v>
+          <t>Columbia</t>
+        </is>
       </c>
       <c r="D4" t="n">
-        <v>1.46</v>
+        <v>0.38</v>
       </c>
       <c r="E4" t="n">
-        <v>0.74</v>
+        <v>0.63</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>N/A</t>
+          <t>Poor</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>2956</v>
+        <v>1172</v>
       </c>
       <c r="J4" t="n">
-        <v>4312</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Columbia</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>0.38</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.63</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Poor</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>1172</v>
-      </c>
-      <c r="J5" t="n">
         <v>738.36</v>
       </c>
     </row>
@@ -518,7 +481,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:K6"/>
+  <dimension ref="B2:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -613,78 +576,27 @@
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>A13</t>
+          <t>F9</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1985</v>
+        <v>2952</v>
       </c>
       <c r="D4" t="n">
-        <v>2.3</v>
+        <v>1.54</v>
       </c>
       <c r="E4" t="n">
-        <v>2.3</v>
+        <v>0.78</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>High</t>
+          <t>Medium</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>833</v>
+        <v>2831</v>
       </c>
       <c r="J4" t="n">
-        <v>3494</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Columbia</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>0.38</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.63</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Poor</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>1172</v>
-      </c>
-      <c r="J5" t="n">
-        <v>738.36</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>F9</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>2952</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1.54</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.78</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Medium</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>2831</v>
-      </c>
-      <c r="J6" t="n">
         <v>4364</v>
       </c>
     </row>
@@ -741,7 +653,7 @@
         <v>1172</v>
       </c>
       <c r="D4" t="n">
-        <v>1172</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -764,7 +676,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2956</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
         <v>2831</v>
@@ -780,7 +692,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>1761</v>
+        <v>928</v>
       </c>
     </row>
     <row r="8">
@@ -829,10 +741,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>4128</v>
+        <v>1172</v>
       </c>
       <c r="D11" t="n">
-        <v>5764</v>
+        <v>3759</v>
       </c>
     </row>
     <row r="14">
@@ -869,7 +781,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -892,7 +804,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
         <v>1</v>
@@ -908,7 +820,7 @@
         <v>1</v>
       </c>
       <c r="D19" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -957,10 +869,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D23" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
group key/values added to VfM
</commit_message>
<xml_diff>
--- a/tests/resources/vfm.xlsx
+++ b/tests/resources/vfm.xlsx
@@ -347,7 +347,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:K4"/>
+  <dimension ref="A2:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -410,63 +410,189 @@
     <row r="3">
       <c r="B3" t="inlineStr">
         <is>
+          <t>Mars</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>28369</v>
+      </c>
+      <c r="D3" t="n">
+        <v>14.58</v>
+      </c>
+      <c r="E3" t="n">
+        <v>12.98</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Very High</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Very High</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Very High</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>2089</v>
+      </c>
+      <c r="J3" t="n">
+        <v>30458</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">All you need is love, love is all you need </t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Roads Places and Environment Group</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>SoT</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C4" t="n">
         <v>1469.2</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D4" t="n">
         <v>2.58</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E4" t="n">
         <v>1.36</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>928 -678</t>
         </is>
       </c>
-      <c r="J3" t="n">
+      <c r="J4" t="n">
         <v>2398</v>
       </c>
     </row>
-    <row r="4">
-      <c r="B4" t="inlineStr">
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>HSMRPG</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>A13</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1985</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>833</v>
+      </c>
+      <c r="J5" t="n">
+        <v>3494</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Rail Group</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>F9</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1356</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.46</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>2956</v>
+      </c>
+      <c r="J6" t="n">
+        <v>4312</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Roads Places and Environment Group</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>Columbia</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="D7" t="n">
         <v>0.38</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E7" t="n">
         <v>0.63</v>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>Poor</t>
         </is>
       </c>
-      <c r="I4" t="n">
+      <c r="I7" t="n">
         <v>1172</v>
       </c>
-      <c r="J4" t="n">
+      <c r="J7" t="n">
         <v>738.36</v>
       </c>
     </row>
@@ -481,7 +607,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:K4"/>
+  <dimension ref="A2:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,60 +670,175 @@
     <row r="3">
       <c r="B3" t="inlineStr">
         <is>
+          <t>Mars</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>30292.2</v>
+      </c>
+      <c r="D3" t="n">
+        <v>21.45</v>
+      </c>
+      <c r="E3" t="n">
+        <v>19.72</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Very High</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>1481.6</v>
+      </c>
+      <c r="J3" t="n">
+        <v>31773.8</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Hello is it me you’re looking for</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Roads Places and Environment Group</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>SoT</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="C4" t="n">
         <v>1469.2</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D4" t="n">
         <v>2.58</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E4" t="n">
         <v>1.36</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>High</t>
         </is>
       </c>
-      <c r="I3" t="n">
+      <c r="I4" t="n">
         <v>928</v>
       </c>
-      <c r="J3" t="n">
+      <c r="J4" t="n">
         <v>2398</v>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="K4" t="inlineStr">
         <is>
           <t>Please allow me to introduce myself I’m a man of wealth and taste.</t>
         </is>
       </c>
     </row>
-    <row r="4">
-      <c r="B4" t="inlineStr">
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>HSMRPG</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>A11</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Rail Group</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>A13</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>1985</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>833</v>
+      </c>
+      <c r="J6" t="n">
+        <v>3494</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Roads Places and Environment Group</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>F9</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C7" t="n">
         <v>2952</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D7" t="n">
         <v>1.54</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E7" t="n">
         <v>0.78</v>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>Medium</t>
         </is>
       </c>
-      <c r="I4" t="n">
+      <c r="I7" t="n">
         <v>2831</v>
       </c>
-      <c r="J4" t="n">
+      <c r="J7" t="n">
         <v>4364</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Rail Group</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Columbia</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Poor</t>
+        </is>
+      </c>
+      <c r="I8" t="n">
+        <v>1172</v>
+      </c>
+      <c r="J8" t="n">
+        <v>738.36</v>
       </c>
     </row>
   </sheetData>
@@ -653,7 +894,7 @@
         <v>1172</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="5">
@@ -676,7 +917,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>2956</v>
       </c>
       <c r="D6" t="n">
         <v>2831</v>
@@ -689,10 +930,10 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>833</v>
       </c>
       <c r="D7" t="n">
-        <v>928</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="8">
@@ -702,10 +943,10 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>2089</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>1481.6</v>
       </c>
     </row>
     <row r="9">
@@ -741,10 +982,10 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1172</v>
+        <v>7050</v>
       </c>
       <c r="D11" t="n">
-        <v>3759</v>
+        <v>7245.6</v>
       </c>
     </row>
     <row r="14">
@@ -781,7 +1022,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -804,7 +1045,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" t="n">
         <v>1</v>
@@ -817,10 +1058,10 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -830,10 +1071,10 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -869,10 +1110,10 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D23" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>